<commit_message>
tinggal 1 modul lagi
</commit_message>
<xml_diff>
--- a/Test Case.xlsx
+++ b/Test Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Demoblaze-playwright\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52CE66F-6CE6-46C2-923D-7F5836352F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C0ED4C-9026-4DA9-BEFD-25C86E2F4F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="1" xr2:uid="{739BE312-AA31-4B31-A566-DB081319E3AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{739BE312-AA31-4B31-A566-DB081319E3AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="260">
   <si>
     <t xml:space="preserve">Pre-condition:  </t>
   </si>
@@ -2222,7 +2222,7 @@
   </sheetPr>
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C78" sqref="C78:C85"/>
     </sheetView>
   </sheetViews>
@@ -3523,14 +3523,14 @@
   </sheetPr>
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45:K48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65:K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="9" max="9" width="20.21875" customWidth="1"/>
@@ -4580,8 +4580,8 @@
         <v>64</v>
       </c>
       <c r="O49" s="47"/>
-      <c r="P49" s="75" t="s">
-        <v>229</v>
+      <c r="P49" s="106" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
@@ -4600,7 +4600,7 @@
       <c r="M50" s="50"/>
       <c r="N50" s="48"/>
       <c r="O50" s="50"/>
-      <c r="P50" s="76"/>
+      <c r="P50" s="107"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="76"/>
@@ -4618,7 +4618,7 @@
       <c r="M51" s="50"/>
       <c r="N51" s="48"/>
       <c r="O51" s="50"/>
-      <c r="P51" s="76"/>
+      <c r="P51" s="107"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="77"/>
@@ -4636,7 +4636,7 @@
       <c r="M52" s="53"/>
       <c r="N52" s="51"/>
       <c r="O52" s="53"/>
-      <c r="P52" s="77"/>
+      <c r="P52" s="108"/>
     </row>
     <row r="53" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="75">
@@ -4670,8 +4670,8 @@
         <v>70</v>
       </c>
       <c r="O53" s="47"/>
-      <c r="P53" s="75" t="s">
-        <v>229</v>
+      <c r="P53" s="106" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
@@ -4690,7 +4690,7 @@
       <c r="M54" s="50"/>
       <c r="N54" s="48"/>
       <c r="O54" s="50"/>
-      <c r="P54" s="76"/>
+      <c r="P54" s="107"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="76"/>
@@ -4708,7 +4708,7 @@
       <c r="M55" s="50"/>
       <c r="N55" s="48"/>
       <c r="O55" s="50"/>
-      <c r="P55" s="76"/>
+      <c r="P55" s="107"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="77"/>
@@ -4726,7 +4726,7 @@
       <c r="M56" s="53"/>
       <c r="N56" s="51"/>
       <c r="O56" s="53"/>
-      <c r="P56" s="77"/>
+      <c r="P56" s="108"/>
     </row>
     <row r="57" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="75">
@@ -5813,7 +5813,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F20"/>
+      <selection activeCell="F21" sqref="F21:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6040,7 +6040,9 @@
       <c r="G17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="20"/>
+      <c r="H17" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="76"/>
@@ -6052,7 +6054,9 @@
       <c r="G18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="20"/>
+      <c r="H18" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="76"/>
@@ -6064,7 +6068,9 @@
       <c r="G19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="20"/>
+      <c r="H19" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="77"/>
@@ -6076,7 +6082,9 @@
       <c r="G20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="20"/>
+      <c r="H20" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="75">
@@ -6096,7 +6104,9 @@
       <c r="G21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="76"/>
@@ -6108,7 +6118,9 @@
       <c r="G22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="20"/>
+      <c r="H22" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="76"/>
@@ -6120,7 +6132,9 @@
       <c r="G23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="20"/>
+      <c r="H23" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="76"/>
@@ -6132,7 +6146,9 @@
       <c r="G24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="77"/>
@@ -6144,7 +6160,9 @@
       <c r="G25" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="1"/>
+      <c r="H25" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="75">

</xml_diff>